<commit_message>
March 2020 GDP update
</commit_message>
<xml_diff>
--- a/static/data/source/state_gdp.xlsx
+++ b/static/data/source/state_gdp.xlsx
@@ -462,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -476,6 +476,7 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,6 +806,7 @@
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="58" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="10.140625" customWidth="1"/>
+    <col min="61" max="61" width="9" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="15.75" x14ac:dyDescent="0.25">
@@ -1190,7 +1192,9 @@
       <c r="BH5" s="5">
         <v>21542540</v>
       </c>
-      <c r="BI5" s="5"/>
+      <c r="BI5" s="5">
+        <v>21615055.070713539</v>
+      </c>
     </row>
     <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1373,6 +1377,9 @@
       <c r="BH6" s="5">
         <v>232144.7</v>
       </c>
+      <c r="BI6" s="5">
+        <v>232687.33251337</v>
+      </c>
     </row>
     <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1555,6 +1562,9 @@
       <c r="BH7" s="5">
         <v>55429.599999999999</v>
       </c>
+      <c r="BI7" s="5">
+        <v>55698.832134022472</v>
+      </c>
     </row>
     <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1737,6 +1747,9 @@
       <c r="BH8" s="5">
         <v>368556.3</v>
       </c>
+      <c r="BI8" s="5">
+        <v>369513.4989075776</v>
+      </c>
     </row>
     <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1919,6 +1932,9 @@
       <c r="BH9" s="5">
         <v>134022.1</v>
       </c>
+      <c r="BI9" s="5">
+        <v>134417.37337832231</v>
+      </c>
     </row>
     <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -2101,6 +2117,9 @@
       <c r="BH10" s="5">
         <v>3155223.7</v>
       </c>
+      <c r="BI10" s="5">
+        <v>3166244.0048968797</v>
+      </c>
     </row>
     <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -2283,6 +2302,9 @@
       <c r="BH11" s="5">
         <v>392347.5</v>
       </c>
+      <c r="BI11" s="5">
+        <v>393855.40061828779</v>
+      </c>
     </row>
     <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -2465,6 +2487,9 @@
       <c r="BH12" s="5">
         <v>287560.09999999998</v>
       </c>
+      <c r="BI12" s="5">
+        <v>288322.54377589922</v>
+      </c>
     </row>
     <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -2647,6 +2672,9 @@
       <c r="BH13" s="5">
         <v>75765.399999999994</v>
       </c>
+      <c r="BI13" s="5">
+        <v>75976.249908918224</v>
+      </c>
     </row>
     <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -2829,6 +2857,9 @@
       <c r="BH14" s="5">
         <v>146995.5</v>
       </c>
+      <c r="BI14" s="5">
+        <v>147511.42917837453</v>
+      </c>
     </row>
     <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -3011,6 +3042,9 @@
       <c r="BH15" s="5">
         <v>1100721.1000000001</v>
       </c>
+      <c r="BI15" s="5">
+        <v>1104177.8183629615</v>
+      </c>
     </row>
     <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -3193,8 +3227,11 @@
       <c r="BH16" s="5">
         <v>619817.69999999995</v>
       </c>
+      <c r="BI16" s="5">
+        <v>621662.17915206752</v>
+      </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -3375,8 +3412,11 @@
       <c r="BH17" s="5">
         <v>97664.4</v>
       </c>
+      <c r="BI17" s="5">
+        <v>97978.27028315948</v>
+      </c>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -3557,8 +3597,11 @@
       <c r="BH18" s="5">
         <v>81492.7</v>
       </c>
+      <c r="BI18" s="5">
+        <v>81754.266152922966</v>
+      </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -3739,8 +3782,11 @@
       <c r="BH19" s="5">
         <v>901571.9</v>
       </c>
+      <c r="BI19" s="5">
+        <v>904716.06578689406</v>
+      </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -3921,8 +3967,11 @@
       <c r="BH20" s="5">
         <v>379132.8</v>
       </c>
+      <c r="BI20" s="5">
+        <v>380661.80319217202</v>
+      </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -4103,8 +4152,11 @@
       <c r="BH21" s="5">
         <v>195857.9</v>
       </c>
+      <c r="BI21" s="5">
+        <v>196561.0177137501</v>
+      </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -4285,8 +4337,11 @@
       <c r="BH22" s="5">
         <v>174183.2</v>
       </c>
+      <c r="BI22" s="5">
+        <v>174780.18230657873</v>
+      </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -4467,8 +4522,11 @@
       <c r="BH23" s="5">
         <v>215585.5</v>
       </c>
+      <c r="BI23" s="5">
+        <v>216346.50508646999</v>
+      </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -4649,8 +4707,11 @@
       <c r="BH24" s="5">
         <v>264853.3</v>
       </c>
+      <c r="BI24" s="5">
+        <v>266335.03985196055</v>
+      </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -4831,8 +4892,11 @@
       <c r="BH25" s="5">
         <v>67905.3</v>
       </c>
+      <c r="BI25" s="5">
+        <v>68117.57703692402</v>
+      </c>
     </row>
-    <row r="26" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
@@ -5013,8 +5077,11 @@
       <c r="BH26" s="5">
         <v>430388.3</v>
       </c>
+      <c r="BI26" s="5">
+        <v>431684.48804295692</v>
+      </c>
     </row>
-    <row r="27" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -5195,8 +5262,11 @@
       <c r="BH27" s="5">
         <v>599091.6</v>
       </c>
+      <c r="BI27" s="5">
+        <v>601058.98485526035</v>
+      </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -5377,8 +5447,11 @@
       <c r="BH28" s="5">
         <v>543976.5</v>
       </c>
+      <c r="BI28" s="5">
+        <v>545450.96762934211</v>
+      </c>
     </row>
-    <row r="29" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -5559,8 +5632,11 @@
       <c r="BH29" s="5">
         <v>383093.6</v>
       </c>
+      <c r="BI29" s="5">
+        <v>384364.71177064546</v>
+      </c>
     </row>
-    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -5741,8 +5817,11 @@
       <c r="BH30" s="5">
         <v>119497.1</v>
       </c>
+      <c r="BI30" s="5">
+        <v>119804.460413623</v>
+      </c>
     </row>
-    <row r="31" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -5923,8 +6002,11 @@
       <c r="BH31" s="5">
         <v>334286.09999999998</v>
       </c>
+      <c r="BI31" s="5">
+        <v>335327.81670043548</v>
+      </c>
     </row>
-    <row r="32" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -6105,8 +6187,11 @@
       <c r="BH32" s="5">
         <v>52470.1</v>
       </c>
+      <c r="BI32" s="5">
+        <v>52660.225288685637</v>
+      </c>
     </row>
-    <row r="33" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
@@ -6287,8 +6372,11 @@
       <c r="BH33" s="5">
         <v>127940.6</v>
       </c>
+      <c r="BI33" s="5">
+        <v>128286.51164637374</v>
+      </c>
     </row>
-    <row r="34" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -6469,8 +6557,11 @@
       <c r="BH34" s="5">
         <v>178621.7</v>
       </c>
+      <c r="BI34" s="5">
+        <v>179307.13121588583</v>
+      </c>
     </row>
-    <row r="35" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
@@ -6651,8 +6742,11 @@
       <c r="BH35" s="5">
         <v>89152.2</v>
       </c>
+      <c r="BI35" s="5">
+        <v>89403.121473631531</v>
+      </c>
     </row>
-    <row r="36" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
@@ -6833,8 +6927,11 @@
       <c r="BH36" s="5">
         <v>648984</v>
       </c>
+      <c r="BI36" s="5">
+        <v>651226.66127221182</v>
+      </c>
     </row>
-    <row r="37" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
@@ -7015,8 +7112,11 @@
       <c r="BH37" s="5">
         <v>104349.4</v>
       </c>
+      <c r="BI37" s="5">
+        <v>104749.77166684542</v>
+      </c>
     </row>
-    <row r="38" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
@@ -7197,8 +7297,11 @@
       <c r="BH38" s="5">
         <v>1740745.3</v>
       </c>
+      <c r="BI38" s="5">
+        <v>1745503.610223884</v>
+      </c>
     </row>
-    <row r="39" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -7379,8 +7482,11 @@
       <c r="BH39" s="5">
         <v>590710.5</v>
       </c>
+      <c r="BI39" s="5">
+        <v>592925.57817749924</v>
+      </c>
     </row>
-    <row r="40" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -7561,8 +7667,11 @@
       <c r="BH40" s="5">
         <v>57106.400000000001</v>
       </c>
+      <c r="BI40" s="5">
+        <v>57334.949116567659</v>
+      </c>
     </row>
-    <row r="41" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -7743,8 +7852,11 @@
       <c r="BH41" s="5">
         <v>701438.5</v>
       </c>
+      <c r="BI41" s="5">
+        <v>703943.0180617664</v>
+      </c>
     </row>
-    <row r="42" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -7925,8 +8037,11 @@
       <c r="BH42" s="5">
         <v>206254</v>
       </c>
+      <c r="BI42" s="5">
+        <v>207094.42957078674</v>
+      </c>
     </row>
-    <row r="43" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -8107,8 +8222,11 @@
       <c r="BH43" s="5">
         <v>253036.4</v>
       </c>
+      <c r="BI43" s="5">
+        <v>253878.98285683151</v>
+      </c>
     </row>
-    <row r="44" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
@@ -8289,8 +8407,11 @@
       <c r="BH44" s="5">
         <v>817216</v>
       </c>
+      <c r="BI44" s="5">
+        <v>820263.20260510012</v>
+      </c>
     </row>
-    <row r="45" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -8471,8 +8592,11 @@
       <c r="BH45" s="5">
         <v>63903.5</v>
       </c>
+      <c r="BI45" s="5">
+        <v>64092.007311210895</v>
+      </c>
     </row>
-    <row r="46" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>42</v>
       </c>
@@ -8653,8 +8777,11 @@
       <c r="BH46" s="5">
         <v>247710.6</v>
       </c>
+      <c r="BI46" s="5">
+        <v>248406.2682073765</v>
+      </c>
     </row>
-    <row r="47" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
@@ -8835,8 +8962,11 @@
       <c r="BH47" s="5">
         <v>53692.3</v>
       </c>
+      <c r="BI47" s="5">
+        <v>53838.331392839355</v>
+      </c>
     </row>
-    <row r="48" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
@@ -9017,8 +9147,11 @@
       <c r="BH48" s="5">
         <v>382274.8</v>
       </c>
+      <c r="BI48" s="5">
+        <v>383803.60903240636</v>
+      </c>
     </row>
-    <row r="49" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -9199,8 +9332,11 @@
       <c r="BH49" s="5">
         <v>1896062.9</v>
       </c>
+      <c r="BI49" s="5">
+        <v>1904246.4107856348</v>
+      </c>
     </row>
-    <row r="50" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>46</v>
       </c>
@@ -9381,8 +9517,11 @@
       <c r="BH50" s="5">
         <v>189809.5</v>
       </c>
+      <c r="BI50" s="5">
+        <v>190404.36157781427</v>
+      </c>
     </row>
-    <row r="51" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -9563,8 +9702,11 @@
       <c r="BH51" s="5">
         <v>34973.5</v>
       </c>
+      <c r="BI51" s="5">
+        <v>35074.224109058065</v>
+      </c>
     </row>
-    <row r="52" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>48</v>
       </c>
@@ -9745,8 +9887,11 @@
       <c r="BH52" s="5">
         <v>557143.9</v>
       </c>
+      <c r="BI52" s="5">
+        <v>558995.19537569105</v>
+      </c>
     </row>
-    <row r="53" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
@@ -9927,8 +10072,11 @@
       <c r="BH53" s="5">
         <v>603772.4</v>
       </c>
+      <c r="BI53" s="5">
+        <v>605344.7969020512</v>
+      </c>
     </row>
-    <row r="54" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
@@ -10109,8 +10257,11 @@
       <c r="BH54" s="5">
         <v>78270.100000000006</v>
       </c>
+      <c r="BI54" s="5">
+        <v>78533.941764542062</v>
+      </c>
     </row>
-    <row r="55" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -10291,8 +10442,11 @@
       <c r="BH55" s="5">
         <v>348822</v>
       </c>
+      <c r="BI55" s="5">
+        <v>350062.63337402546</v>
+      </c>
     </row>
-    <row r="56" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
@@ -10472,6 +10626,9 @@
       </c>
       <c r="BH56" s="5">
         <v>39610.5</v>
+      </c>
+      <c r="BI56" s="5">
+        <v>39793.125113670663</v>
       </c>
     </row>
   </sheetData>
@@ -10494,6 +10651,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="57" max="57" width="8" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="15.75" x14ac:dyDescent="0.25">
@@ -10855,6 +11013,9 @@
       <c r="BD5" s="6">
         <v>1.7118099400957678</v>
       </c>
+      <c r="BE5" s="6">
+        <v>1.6062864834873372</v>
+      </c>
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -11025,6 +11186,9 @@
       <c r="BD6" s="6">
         <v>1.9061776968739379</v>
       </c>
+      <c r="BE6" s="6">
+        <v>1.5861291945738327</v>
+      </c>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -11195,6 +11359,9 @@
       <c r="BD7" s="6">
         <v>-2.593669542572302</v>
       </c>
+      <c r="BE7" s="6">
+        <v>-1.8398811688719898</v>
+      </c>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -11365,6 +11532,9 @@
       <c r="BD8" s="6">
         <v>2.0310558330485153</v>
       </c>
+      <c r="BE8" s="6">
+        <v>1.8266441665629312</v>
+      </c>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -11535,6 +11705,9 @@
       <c r="BD9" s="6">
         <v>1.9511247628908059</v>
       </c>
+      <c r="BE9" s="6">
+        <v>1.6525674219260404</v>
+      </c>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -11705,6 +11878,9 @@
       <c r="BD10" s="6">
         <v>2.0977762701282789</v>
       </c>
+      <c r="BE10" s="6">
+        <v>2.0026309578479231</v>
+      </c>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -11875,6 +12051,9 @@
       <c r="BD11" s="6">
         <v>1.1883043684816992</v>
       </c>
+      <c r="BE11" s="6">
+        <v>1.2740012075599947</v>
+      </c>
     </row>
     <row r="12" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -12045,6 +12224,9 @@
       <c r="BD12" s="6">
         <v>2.0701943572557218</v>
       </c>
+      <c r="BE12" s="6">
+        <v>1.8852214909389335</v>
+      </c>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -12215,6 +12397,9 @@
       <c r="BD13" s="6">
         <v>1.8439506771787677</v>
       </c>
+      <c r="BE13" s="6">
+        <v>1.5992196698830794</v>
+      </c>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -12385,6 +12570,9 @@
       <c r="BD14" s="6">
         <v>2.3592513861688116</v>
       </c>
+      <c r="BE14" s="6">
+        <v>2.2367421414254922</v>
+      </c>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -12555,6 +12743,9 @@
       <c r="BD15" s="6">
         <v>2.4917793401049844</v>
       </c>
+      <c r="BE15" s="6">
+        <v>2.230984529274691</v>
+      </c>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -12725,8 +12916,11 @@
       <c r="BD16" s="6">
         <v>2.1675769260629592</v>
       </c>
+      <c r="BE16" s="6">
+        <v>1.9522354115343501</v>
+      </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
@@ -12895,8 +13089,11 @@
       <c r="BD17" s="6">
         <v>2.82866921317139</v>
       </c>
+      <c r="BE17" s="6">
+        <v>2.4502872398924107</v>
+      </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -13065,8 +13262,11 @@
       <c r="BD18" s="6">
         <v>2.4139228846505705</v>
       </c>
+      <c r="BE18" s="6">
+        <v>2.1052215713507358</v>
+      </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -13235,8 +13435,11 @@
       <c r="BD19" s="6">
         <v>2.1380788843686283</v>
       </c>
+      <c r="BE19" s="6">
+        <v>1.9390777891015816</v>
+      </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -13405,8 +13608,11 @@
       <c r="BD20" s="6">
         <v>1.985622116436814</v>
       </c>
+      <c r="BE20" s="6">
+        <v>1.7664820334293783</v>
+      </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -13575,8 +13781,11 @@
       <c r="BD21" s="6">
         <v>1.9914284424529918</v>
       </c>
+      <c r="BE21" s="6">
+        <v>1.7747965696039623</v>
+      </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -13745,8 +13954,11 @@
       <c r="BD22" s="6">
         <v>2.0741599217814635</v>
       </c>
+      <c r="BE22" s="6">
+        <v>1.830527739912414</v>
+      </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
@@ -13915,8 +14127,11 @@
       <c r="BD23" s="6">
         <v>2.0814195150203396</v>
       </c>
+      <c r="BE23" s="6">
+        <v>1.8386319597583731</v>
+      </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
@@ -14085,8 +14300,11 @@
       <c r="BD24" s="6">
         <v>0.70226773512812646</v>
       </c>
+      <c r="BE24" s="6">
+        <v>0.70120119948608139</v>
+      </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -14255,8 +14473,11 @@
       <c r="BD25" s="6">
         <v>2.3519574330503499</v>
       </c>
+      <c r="BE25" s="6">
+        <v>2.0422648264871386</v>
+      </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
@@ -14425,8 +14646,11 @@
       <c r="BD26" s="6">
         <v>2.4233158426556236</v>
       </c>
+      <c r="BE26" s="6">
+        <v>2.1648576307530014</v>
+      </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
@@ -14595,8 +14819,11 @@
       <c r="BD27" s="6">
         <v>2.1016787712013185</v>
       </c>
+      <c r="BE27" s="6">
+        <v>1.9799855641466511</v>
+      </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -14765,8 +14992,11 @@
       <c r="BD28" s="6">
         <v>2.1390665673726295</v>
       </c>
+      <c r="BE28" s="6">
+        <v>1.9026390505064281</v>
+      </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
@@ -14935,8 +15165,11 @@
       <c r="BD29" s="6">
         <v>1.8461557340053487</v>
       </c>
+      <c r="BE29" s="6">
+        <v>1.6820198262403441</v>
+      </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
@@ -15105,8 +15338,11 @@
       <c r="BD30" s="6">
         <v>2.166237517719356</v>
       </c>
+      <c r="BE30" s="6">
+        <v>1.7422188223020381</v>
+      </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>27</v>
       </c>
@@ -15275,8 +15511,11 @@
       <c r="BD31" s="6">
         <v>2.0865996566881315</v>
       </c>
+      <c r="BE31" s="6">
+        <v>1.859953818307561</v>
+      </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>28</v>
       </c>
@@ -15445,8 +15684,11 @@
       <c r="BD32" s="6">
         <v>1.4980042940546219</v>
       </c>
+      <c r="BE32" s="6">
+        <v>1.3784853073905268</v>
+      </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>29</v>
       </c>
@@ -15615,8 +15857,11 @@
       <c r="BD33" s="6">
         <v>2.2009248558920551</v>
       </c>
+      <c r="BE33" s="6">
+        <v>1.827456549627942</v>
+      </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
@@ -15785,8 +16030,11 @@
       <c r="BD34" s="6">
         <v>1.8934924647550437</v>
       </c>
+      <c r="BE34" s="6">
+        <v>1.8469751525091351</v>
+      </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
@@ -15955,8 +16203,11 @@
       <c r="BD35" s="6">
         <v>2.2478804171783215</v>
       </c>
+      <c r="BE35" s="6">
+        <v>2.0286707627955312</v>
+      </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
@@ -16125,8 +16376,11 @@
       <c r="BD36" s="6">
         <v>2.2751153290714923</v>
       </c>
+      <c r="BE36" s="6">
+        <v>2.0703660089105624</v>
+      </c>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
@@ -16295,8 +16549,11 @@
       <c r="BD37" s="6">
         <v>-0.77736965515771894</v>
       </c>
+      <c r="BE37" s="6">
+        <v>-0.35961525215773305</v>
+      </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
@@ -16465,8 +16722,11 @@
       <c r="BD38" s="6">
         <v>1.9901625480709393</v>
       </c>
+      <c r="BE38" s="6">
+        <v>1.8404831980217007</v>
+      </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>35</v>
       </c>
@@ -16635,8 +16895,11 @@
       <c r="BD39" s="6">
         <v>2.0371295404850076</v>
       </c>
+      <c r="BE39" s="6">
+        <v>1.8482586315131757</v>
+      </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>36</v>
       </c>
@@ -16805,8 +17068,11 @@
       <c r="BD40" s="6">
         <v>-1.1575495290435598</v>
       </c>
+      <c r="BE40" s="6">
+        <v>-0.63604711779058287</v>
+      </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -16975,8 +17241,11 @@
       <c r="BD41" s="6">
         <v>1.5062244352679262</v>
       </c>
+      <c r="BE41" s="6">
+        <v>1.3837955784369513</v>
+      </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>38</v>
       </c>
@@ -17145,8 +17414,11 @@
       <c r="BD42" s="6">
         <v>-1.7708703727617154</v>
       </c>
+      <c r="BE42" s="6">
+        <v>-1.1681233735472687</v>
+      </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>39</v>
       </c>
@@ -17315,8 +17587,11 @@
       <c r="BD43" s="6">
         <v>2.3112373008806855</v>
       </c>
+      <c r="BE43" s="6">
+        <v>2.1069228723603426</v>
+      </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>40</v>
       </c>
@@ -17485,8 +17760,11 @@
       <c r="BD44" s="6">
         <v>1.4446369698053461</v>
       </c>
+      <c r="BE44" s="6">
+        <v>1.4121013546463768</v>
+      </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>41</v>
       </c>
@@ -17655,8 +17933,11 @@
       <c r="BD45" s="6">
         <v>2.283865844030442</v>
       </c>
+      <c r="BE45" s="6">
+        <v>2.0366496161046483</v>
+      </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>42</v>
       </c>
@@ -17825,8 +18106,11 @@
       <c r="BD46" s="6">
         <v>2.3359145173955898</v>
       </c>
+      <c r="BE46" s="6">
+        <v>2.0041952370333171</v>
+      </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>43</v>
       </c>
@@ -17995,8 +18279,11 @@
       <c r="BD47" s="6">
         <v>2.1365775149401967</v>
       </c>
+      <c r="BE47" s="6">
+        <v>1.8176307571206323</v>
+      </c>
     </row>
-    <row r="48" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>44</v>
       </c>
@@ -18165,8 +18452,11 @@
       <c r="BD48" s="6">
         <v>2.210030976420982</v>
       </c>
+      <c r="BE48" s="6">
+        <v>2.0349096362214261</v>
+      </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>45</v>
       </c>
@@ -18335,8 +18625,11 @@
       <c r="BD49" s="6">
         <v>-0.47671687061187618</v>
       </c>
+      <c r="BE49" s="6">
+        <v>-0.10964563713568073</v>
+      </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>46</v>
       </c>
@@ -18505,8 +18798,11 @@
       <c r="BD50" s="6">
         <v>1.9011321196383697</v>
       </c>
+      <c r="BE50" s="6">
+        <v>1.720178676330693</v>
+      </c>
     </row>
-    <row r="51" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>47</v>
       </c>
@@ -18675,8 +18971,11 @@
       <c r="BD51" s="6">
         <v>2.221194980293876</v>
       </c>
+      <c r="BE51" s="6">
+        <v>1.9631668630926693</v>
+      </c>
     </row>
-    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>48</v>
       </c>
@@ -18845,8 +19144,11 @@
       <c r="BD52" s="6">
         <v>2.1935374339044591</v>
       </c>
+      <c r="BE52" s="6">
+        <v>1.9965093737900637</v>
+      </c>
     </row>
-    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>49</v>
       </c>
@@ -19015,8 +19317,11 @@
       <c r="BD53" s="6">
         <v>2.1521643174123897</v>
       </c>
+      <c r="BE53" s="6">
+        <v>1.9540068115078773</v>
+      </c>
     </row>
-    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>50</v>
       </c>
@@ -19185,8 +19490,11 @@
       <c r="BD54" s="6">
         <v>-0.59378461618810896</v>
       </c>
+      <c r="BE54" s="6">
+        <v>-0.29391324902558891</v>
+      </c>
     </row>
-    <row r="55" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>51</v>
       </c>
@@ -19355,8 +19663,11 @@
       <c r="BD55" s="6">
         <v>1.9266433768881626</v>
       </c>
+      <c r="BE55" s="6">
+        <v>1.7505031528145174</v>
+      </c>
     </row>
-    <row r="56" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>52</v>
       </c>
@@ -19524,6 +19835,9 @@
       </c>
       <c r="BD56" s="6">
         <v>-3.1824241080328903</v>
+      </c>
+      <c r="BE56" s="6">
+        <v>-2.2320390553512262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>